<commit_message>
FoF summary table added to HFRI_full to simplify new code
</commit_message>
<xml_diff>
--- a/Data/HFRI_full.xlsx
+++ b/Data/HFRI_full.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HEC\MASTER_THESIS\Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Python tools\MasterThesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B339A3-3F5C-4F71-9133-99F9AF69692A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8752382B-B319-432E-AA8B-772F4A62A549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53100" yWindow="4224" windowWidth="20208" windowHeight="20112" xr2:uid="{7F518E60-2123-4967-B68A-67F8C00FD90A}"/>
+    <workbookView xWindow="47004" yWindow="3480" windowWidth="32700" windowHeight="19104" activeTab="1" xr2:uid="{7F518E60-2123-4967-B68A-67F8C00FD90A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Indices" sheetId="1" r:id="rId1"/>
+    <sheet name="FoF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>HFRI Equity Hedge (Total) Index (HFRIEHI)</t>
   </si>
@@ -90,6 +91,48 @@
   </si>
   <si>
     <t>Data Source: Hedge Fund Research Inc. - © 2023 HFR Inc. - www.hfr.com</t>
+  </si>
+  <si>
+    <t>FoF</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>M squared</t>
+  </si>
+  <si>
+    <t>Volatility</t>
+  </si>
+  <si>
+    <t>MDD</t>
+  </si>
+  <si>
+    <t>CVaR</t>
+  </si>
+  <si>
+    <t>CDaR</t>
+  </si>
+  <si>
+    <t>Sharpe</t>
+  </si>
+  <si>
+    <t>Calmar</t>
+  </si>
+  <si>
+    <t>R squared</t>
+  </si>
+  <si>
+    <t>Corr. Stocks</t>
+  </si>
+  <si>
+    <t>Corr. Bonds</t>
+  </si>
+  <si>
+    <t>Corr. FoF</t>
+  </si>
+  <si>
+    <t>Turnover</t>
   </si>
 </sst>
 </file>
@@ -146,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -292,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,7 +487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F5345B-73AC-49BC-8FDC-EA0A6AE50390}">
   <dimension ref="A1:Q414"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
+    <sheetView topLeftCell="G1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -19463,4 +19508,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05207327-FE10-4B8D-B3B7-2BD77327BD60}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>4.9341000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>4.9341000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>5.6390999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>0.22203500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>7.2119000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>0.242259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>0.122638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3.1147000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>0.64783500000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>0.36085899999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added FoF to data to solve FoF benchmark complexity
</commit_message>
<xml_diff>
--- a/Data/HFRI_full.xlsx
+++ b/Data/HFRI_full.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\HEC\MASTER_THESIS\Research\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Python tools\MasterThesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B339A3-3F5C-4F71-9133-99F9AF69692A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD62834A-E7F8-4DB4-A7FE-8C9BD9694E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53100" yWindow="4224" windowWidth="20208" windowHeight="20112" xr2:uid="{7F518E60-2123-4967-B68A-67F8C00FD90A}"/>
+    <workbookView xWindow="4020" yWindow="5232" windowWidth="32700" windowHeight="19104" activeTab="1" xr2:uid="{7F518E60-2123-4967-B68A-67F8C00FD90A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="FoF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>HFRI Equity Hedge (Total) Index (HFRIEHI)</t>
   </si>
@@ -90,6 +91,48 @@
   </si>
   <si>
     <t>Data Source: Hedge Fund Research Inc. - © 2023 HFR Inc. - www.hfr.com</t>
+  </si>
+  <si>
+    <t>FoF</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>M squared</t>
+  </si>
+  <si>
+    <t>Volatility</t>
+  </si>
+  <si>
+    <t>MDD</t>
+  </si>
+  <si>
+    <t>CVaR</t>
+  </si>
+  <si>
+    <t>CDaR</t>
+  </si>
+  <si>
+    <t>Sharpe</t>
+  </si>
+  <si>
+    <t>Calmar</t>
+  </si>
+  <si>
+    <t>R squared</t>
+  </si>
+  <si>
+    <t>Corr. Stocks</t>
+  </si>
+  <si>
+    <t>Corr. Bonds</t>
+  </si>
+  <si>
+    <t>Corr. FoF</t>
+  </si>
+  <si>
+    <t>Turnover</t>
   </si>
 </sst>
 </file>
@@ -146,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -292,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F5345B-73AC-49BC-8FDC-EA0A6AE50390}">
   <dimension ref="A1:Q414"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -19463,4 +19506,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3518BF-8E39-446F-907C-6FFCB1F6E3D0}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>4.9341000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>4.9341000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>5.6390999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>0.22203500000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>7.2119000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>0.242259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <v>0.122638</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>3.1147000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>0.64783500000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>0.36085899999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>